<commit_message>
Add EventSeries Add helper functions in utils.R Addtionally clean-up imported classes and functions from FEMS and FEMSdevBase
</commit_message>
<xml_diff>
--- a/src/data/bankA/ANN_Portfolio.xlsx
+++ b/src/data/bankA/ANN_Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/bankA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24A7A35-1B22-E647-B2CA-7FD151E9F79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEF1B0F-8CE5-3C43-8F6A-8D15A9201FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{2827F415-5853-FE46-AE22-EC4475DFFC5F}"/>
   </bookViews>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF54409-75AA-D240-BC62-D87145E7C900}">
   <dimension ref="A1:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,7 +727,7 @@
     <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
@@ -923,7 +923,7 @@
         <v>44</v>
       </c>
       <c r="Q2" s="1">
-        <f t="shared" ref="Q2:Q23" si="0">U2</f>
+        <f t="shared" ref="Q2:Q16" si="0">U2</f>
         <v>46023</v>
       </c>
       <c r="R2" s="1">
@@ -943,7 +943,7 @@
       </c>
       <c r="V2">
         <f ca="1">RANDBETWEEN(500000, 3000000)</f>
-        <v>1737661</v>
+        <v>2808053</v>
       </c>
       <c r="W2" s="1">
         <f>DATE(YEAR(S2)+1,MONTH(S2),DAY(S2))</f>
@@ -1046,7 +1046,7 @@
         <v>46753</v>
       </c>
       <c r="R3" s="1">
-        <f t="shared" ref="R3:R23" si="2">E3</f>
+        <f t="shared" ref="R3:R16" si="2">E3</f>
         <v>44561</v>
       </c>
       <c r="S3" s="1">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V16" ca="1" si="4">RANDBETWEEN(500000, 3000000)</f>
-        <v>2721605</v>
+        <v>1923641</v>
       </c>
       <c r="W3" s="1">
         <f t="shared" ref="W3:W16" si="5">DATE(YEAR(S3)+1,MONTH(S3),DAY(S3))</f>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="4"/>
-        <v>2335062</v>
+        <v>1539561</v>
       </c>
       <c r="W4" s="1">
         <f t="shared" si="5"/>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="V5">
         <f t="shared" ca="1" si="4"/>
-        <v>2277854</v>
+        <v>2981112</v>
       </c>
       <c r="W5" s="1">
         <f t="shared" si="5"/>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="V6">
         <f t="shared" ca="1" si="4"/>
-        <v>2307540</v>
+        <v>2297536</v>
       </c>
       <c r="W6" s="1">
         <f t="shared" si="5"/>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="V7">
         <f t="shared" ca="1" si="4"/>
-        <v>1990634</v>
+        <v>1729008</v>
       </c>
       <c r="W7" s="1">
         <f t="shared" si="5"/>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="V8">
         <f t="shared" ca="1" si="4"/>
-        <v>1144671</v>
+        <v>992005</v>
       </c>
       <c r="W8" s="1">
         <f t="shared" si="5"/>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="V9">
         <f t="shared" ca="1" si="4"/>
-        <v>1924996</v>
+        <v>2707766</v>
       </c>
       <c r="W9" s="1">
         <f t="shared" si="5"/>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="V10">
         <f t="shared" ca="1" si="4"/>
-        <v>2255822</v>
+        <v>2487277</v>
       </c>
       <c r="W10" s="1">
         <f t="shared" si="5"/>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="V11">
         <f t="shared" ca="1" si="4"/>
-        <v>728355</v>
+        <v>2210409</v>
       </c>
       <c r="W11" s="1">
         <f t="shared" si="5"/>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="V12">
         <f t="shared" ca="1" si="4"/>
-        <v>2319221</v>
+        <v>2953374</v>
       </c>
       <c r="W12" s="1">
         <f t="shared" si="5"/>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="V13">
         <f t="shared" ca="1" si="4"/>
-        <v>530676</v>
+        <v>899707</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" si="5"/>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="V14">
         <f t="shared" ca="1" si="4"/>
-        <v>1467807</v>
+        <v>648554</v>
       </c>
       <c r="W14" s="1">
         <f t="shared" si="5"/>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="V15">
         <f t="shared" ca="1" si="4"/>
-        <v>2377417</v>
+        <v>2117564</v>
       </c>
       <c r="W15" s="1">
         <f t="shared" si="5"/>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="V16">
         <f t="shared" ca="1" si="4"/>
-        <v>1780521</v>
+        <v>665165</v>
       </c>
       <c r="W16" s="1">
         <f t="shared" si="5"/>
@@ -2680,11 +2680,11 @@
         <v>44</v>
       </c>
       <c r="Q17" s="1">
-        <f>U17</f>
+        <f t="shared" ref="Q17:Q28" si="9">U17</f>
         <v>45292</v>
       </c>
       <c r="R17" s="1">
-        <f>E17</f>
+        <f t="shared" ref="R17:R23" si="10">E17</f>
         <v>44561</v>
       </c>
       <c r="S17" s="1">
@@ -2794,11 +2794,11 @@
         <v>44</v>
       </c>
       <c r="Q18" s="1">
-        <f>U18</f>
+        <f t="shared" si="9"/>
         <v>46388</v>
       </c>
       <c r="R18" s="1">
-        <f>E18</f>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S18" s="1">
@@ -2816,7 +2816,7 @@
         <v>550000</v>
       </c>
       <c r="W18" s="1">
-        <f t="shared" ref="W18:W23" si="9">DATE(YEAR(S18)+1,MONTH(S18),DAY(S18))</f>
+        <f t="shared" ref="W18:W23" si="11">DATE(YEAR(S18)+1,MONTH(S18),DAY(S18))</f>
         <v>44927</v>
       </c>
       <c r="X18" t="s">
@@ -2829,7 +2829,7 @@
         <v>37</v>
       </c>
       <c r="AA18" s="1">
-        <f t="shared" ref="AA18:AA20" si="10">R18</f>
+        <f t="shared" ref="AA18:AA20" si="12">R18</f>
         <v>44561</v>
       </c>
       <c r="AB18" t="s">
@@ -2912,11 +2912,11 @@
         <v>44</v>
       </c>
       <c r="Q19" s="1">
-        <f>U19</f>
+        <f t="shared" si="9"/>
         <v>46023</v>
       </c>
       <c r="R19" s="1">
-        <f>E19</f>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S19" s="1">
@@ -2934,7 +2934,7 @@
         <v>725000</v>
       </c>
       <c r="W19" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X19" t="s">
@@ -2947,7 +2947,7 @@
         <v>37</v>
       </c>
       <c r="AA19" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>44561</v>
       </c>
       <c r="AB19" t="s">
@@ -3030,11 +3030,11 @@
         <v>44</v>
       </c>
       <c r="Q20" s="1">
-        <f>U20</f>
+        <f t="shared" si="9"/>
         <v>47119</v>
       </c>
       <c r="R20" s="1">
-        <f>E20</f>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S20" s="1">
@@ -3052,7 +3052,7 @@
         <v>225000</v>
       </c>
       <c r="W20" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X20" t="s">
@@ -3065,7 +3065,7 @@
         <v>37</v>
       </c>
       <c r="AA20" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>44561</v>
       </c>
       <c r="AB20" t="s">
@@ -3148,11 +3148,11 @@
         <v>44</v>
       </c>
       <c r="Q21" s="1">
-        <f>U21</f>
+        <f t="shared" si="9"/>
         <v>46753</v>
       </c>
       <c r="R21" s="1">
-        <f>E21</f>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S21" s="1">
@@ -3170,7 +3170,7 @@
         <v>500000</v>
       </c>
       <c r="W21" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X21" t="s">
@@ -3240,7 +3240,7 @@
         <v>98</v>
       </c>
       <c r="J22" s="3">
-        <f t="shared" ref="J22:J28" si="11">DATE(YEAR(S22)+1,MONTH(S22),DAY(S22))</f>
+        <f t="shared" ref="J22:J28" si="13">DATE(YEAR(S22)+1,MONTH(S22),DAY(S22))</f>
         <v>44927</v>
       </c>
       <c r="K22" t="s">
@@ -3262,11 +3262,11 @@
         <v>44</v>
       </c>
       <c r="Q22" s="1">
-        <f>U22</f>
+        <f t="shared" si="9"/>
         <v>48214</v>
       </c>
       <c r="R22" s="1">
-        <f>E22</f>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S22" s="1">
@@ -3284,7 +3284,7 @@
         <v>1450000</v>
       </c>
       <c r="W22" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X22" t="s">
@@ -3354,7 +3354,7 @@
         <v>98</v>
       </c>
       <c r="J23" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44927</v>
       </c>
       <c r="K23" t="s">
@@ -3376,11 +3376,11 @@
         <v>44</v>
       </c>
       <c r="Q23" s="1">
-        <f>U23</f>
+        <f t="shared" si="9"/>
         <v>47484</v>
       </c>
       <c r="R23" s="1">
-        <f>E23</f>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S23" s="1">
@@ -3398,7 +3398,7 @@
         <v>550000</v>
       </c>
       <c r="W23" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X23" t="s">
@@ -3411,7 +3411,7 @@
         <v>37</v>
       </c>
       <c r="AA23" s="1">
-        <f t="shared" ref="AA23:AA25" si="12">R23</f>
+        <f t="shared" ref="AA23:AA25" si="14">R23</f>
         <v>44561</v>
       </c>
       <c r="AB23" t="s">
@@ -3472,7 +3472,7 @@
         <v>98</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44927</v>
       </c>
       <c r="K24" t="s">
@@ -3494,11 +3494,11 @@
         <v>44</v>
       </c>
       <c r="Q24" s="1">
-        <f>U24</f>
+        <f t="shared" si="9"/>
         <v>46388</v>
       </c>
       <c r="R24" s="1">
-        <f t="shared" ref="R24:R28" si="13">E24</f>
+        <f t="shared" ref="R24:R28" si="15">E24</f>
         <v>44561</v>
       </c>
       <c r="S24" s="1">
@@ -3516,7 +3516,7 @@
         <v>1500000</v>
       </c>
       <c r="W24" s="1">
-        <f t="shared" ref="W24:W28" si="14">DATE(YEAR(S24)+1,MONTH(S24),DAY(S24))</f>
+        <f t="shared" ref="W24:W28" si="16">DATE(YEAR(S24)+1,MONTH(S24),DAY(S24))</f>
         <v>44927</v>
       </c>
       <c r="X24" t="s">
@@ -3529,7 +3529,7 @@
         <v>37</v>
       </c>
       <c r="AA24" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>44561</v>
       </c>
       <c r="AB24" t="s">
@@ -3590,7 +3590,7 @@
         <v>98</v>
       </c>
       <c r="J25" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44927</v>
       </c>
       <c r="K25" t="s">
@@ -3612,11 +3612,11 @@
         <v>44</v>
       </c>
       <c r="Q25" s="1">
-        <f>U25</f>
+        <f t="shared" si="9"/>
         <v>48214</v>
       </c>
       <c r="R25" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>44561</v>
       </c>
       <c r="S25" s="1">
@@ -3634,20 +3634,20 @@
         <v>3500000</v>
       </c>
       <c r="W25" s="1">
+        <f t="shared" si="16"/>
+        <v>44927</v>
+      </c>
+      <c r="X25" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA25" s="1">
         <f t="shared" si="14"/>
-        <v>44927</v>
-      </c>
-      <c r="X25" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA25" s="1">
-        <f t="shared" si="12"/>
         <v>44561</v>
       </c>
       <c r="AB25" t="s">
@@ -3708,7 +3708,7 @@
         <v>98</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44927</v>
       </c>
       <c r="K26" t="s">
@@ -3730,11 +3730,11 @@
         <v>44</v>
       </c>
       <c r="Q26" s="1">
-        <f>U26</f>
+        <f t="shared" si="9"/>
         <v>47119</v>
       </c>
       <c r="R26" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>44561</v>
       </c>
       <c r="S26" s="1">
@@ -3752,7 +3752,7 @@
         <v>2000000</v>
       </c>
       <c r="W26" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>44927</v>
       </c>
       <c r="X26" t="s">
@@ -3822,7 +3822,7 @@
         <v>98</v>
       </c>
       <c r="J27" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44927</v>
       </c>
       <c r="K27" t="s">
@@ -3844,11 +3844,11 @@
         <v>44</v>
       </c>
       <c r="Q27" s="1">
-        <f>U27</f>
+        <f t="shared" si="9"/>
         <v>45292</v>
       </c>
       <c r="R27" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>44561</v>
       </c>
       <c r="S27" s="1">
@@ -3866,7 +3866,7 @@
         <v>1250000</v>
       </c>
       <c r="W27" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>44927</v>
       </c>
       <c r="X27" t="s">
@@ -3936,7 +3936,7 @@
         <v>98</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>44927</v>
       </c>
       <c r="K28" t="s">
@@ -3958,11 +3958,11 @@
         <v>44</v>
       </c>
       <c r="Q28" s="1">
-        <f>U28</f>
+        <f t="shared" si="9"/>
         <v>45658</v>
       </c>
       <c r="R28" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>44561</v>
       </c>
       <c r="S28" s="1">
@@ -3980,7 +3980,7 @@
         <v>1750000</v>
       </c>
       <c r="W28" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>44927</v>
       </c>
       <c r="X28" t="s">
@@ -3993,7 +3993,7 @@
         <v>37</v>
       </c>
       <c r="AA28" s="1">
-        <f t="shared" ref="AA28" si="15">R28</f>
+        <f t="shared" ref="AA28" si="17">R28</f>
         <v>44561</v>
       </c>
       <c r="AB28" t="s">

</xml_diff>

<commit_message>
change date format in ann ptf
</commit_message>
<xml_diff>
--- a/src/data/bankA/ANN_Portfolio.xlsx
+++ b/src/data/bankA/ANN_Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/bankA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEF1B0F-8CE5-3C43-8F6A-8D15A9201FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B126D1B-46FE-9A4E-A075-BA8E4FAB5FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{2827F415-5853-FE46-AE22-EC4475DFFC5F}"/>
   </bookViews>
@@ -395,11 +395,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -717,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF54409-75AA-D240-BC62-D87145E7C900}">
   <dimension ref="A1:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -900,7 +899,7 @@
       <c r="I2" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="1">
         <f>DATE(YEAR(S2)+1,MONTH(S2),DAY(S2))</f>
         <v>44927</v>
       </c>
@@ -943,7 +942,7 @@
       </c>
       <c r="V2">
         <f ca="1">RANDBETWEEN(500000, 3000000)</f>
-        <v>2808053</v>
+        <v>1668220</v>
       </c>
       <c r="W2" s="1">
         <f>DATE(YEAR(S2)+1,MONTH(S2),DAY(S2))</f>
@@ -1019,7 +1018,7 @@
       <c r="I3" t="s">
         <v>98</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="1">
         <f>DATE(YEAR(S3),MONTH(S3)+6,DAY(S3))</f>
         <v>44743</v>
       </c>
@@ -1062,7 +1061,7 @@
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V16" ca="1" si="4">RANDBETWEEN(500000, 3000000)</f>
-        <v>1923641</v>
+        <v>509310</v>
       </c>
       <c r="W3" s="1">
         <f t="shared" ref="W3:W16" si="5">DATE(YEAR(S3)+1,MONTH(S3),DAY(S3))</f>
@@ -1138,7 +1137,7 @@
       <c r="I4" t="s">
         <v>98</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="1">
         <f t="shared" ref="J4:J21" si="7">DATE(YEAR(S4)+1,MONTH(S4),DAY(S4))</f>
         <v>44927</v>
       </c>
@@ -1181,7 +1180,7 @@
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="4"/>
-        <v>1539561</v>
+        <v>2193970</v>
       </c>
       <c r="W4" s="1">
         <f t="shared" si="5"/>
@@ -1257,7 +1256,7 @@
       <c r="I5" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -1300,7 +1299,7 @@
       </c>
       <c r="V5">
         <f t="shared" ca="1" si="4"/>
-        <v>2981112</v>
+        <v>2394700</v>
       </c>
       <c r="W5" s="1">
         <f t="shared" si="5"/>
@@ -1372,7 +1371,7 @@
       <c r="I6" t="s">
         <v>98</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -1415,7 +1414,7 @@
       </c>
       <c r="V6">
         <f t="shared" ca="1" si="4"/>
-        <v>2297536</v>
+        <v>661056</v>
       </c>
       <c r="W6" s="1">
         <f t="shared" si="5"/>
@@ -1487,7 +1486,7 @@
       <c r="I7" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="1">
         <f>DATE(YEAR(S7),MONTH(S7)+3,DAY(S7))</f>
         <v>44652</v>
       </c>
@@ -1530,7 +1529,7 @@
       </c>
       <c r="V7">
         <f t="shared" ca="1" si="4"/>
-        <v>1729008</v>
+        <v>1792442</v>
       </c>
       <c r="W7" s="1">
         <f t="shared" si="5"/>
@@ -1602,7 +1601,7 @@
       <c r="I8" t="s">
         <v>98</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="1">
         <f>DATE(YEAR(S8),MONTH(S8)+6,DAY(S8))</f>
         <v>44743</v>
       </c>
@@ -1645,7 +1644,7 @@
       </c>
       <c r="V8">
         <f t="shared" ca="1" si="4"/>
-        <v>992005</v>
+        <v>694105</v>
       </c>
       <c r="W8" s="1">
         <f t="shared" si="5"/>
@@ -1721,7 +1720,7 @@
       <c r="I9" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="1">
         <f>DATE(YEAR(S9),MONTH(S9)+1,DAY(S9))</f>
         <v>44593</v>
       </c>
@@ -1764,7 +1763,7 @@
       </c>
       <c r="V9">
         <f t="shared" ca="1" si="4"/>
-        <v>2707766</v>
+        <v>2715929</v>
       </c>
       <c r="W9" s="1">
         <f t="shared" si="5"/>
@@ -1840,7 +1839,7 @@
       <c r="I10" t="s">
         <v>98</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="1">
         <f t="shared" ref="J10:J14" si="8">DATE(YEAR(S10),MONTH(S10)+1,DAY(S10))</f>
         <v>44593</v>
       </c>
@@ -1883,7 +1882,7 @@
       </c>
       <c r="V10">
         <f t="shared" ca="1" si="4"/>
-        <v>2487277</v>
+        <v>2059337</v>
       </c>
       <c r="W10" s="1">
         <f t="shared" si="5"/>
@@ -1955,7 +1954,7 @@
       <c r="I11" t="s">
         <v>98</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="1">
         <f t="shared" si="8"/>
         <v>44593</v>
       </c>
@@ -1998,7 +1997,7 @@
       </c>
       <c r="V11">
         <f t="shared" ca="1" si="4"/>
-        <v>2210409</v>
+        <v>920658</v>
       </c>
       <c r="W11" s="1">
         <f t="shared" si="5"/>
@@ -2074,7 +2073,7 @@
       <c r="I12" t="s">
         <v>98</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -2117,7 +2116,7 @@
       </c>
       <c r="V12">
         <f t="shared" ca="1" si="4"/>
-        <v>2953374</v>
+        <v>1542273</v>
       </c>
       <c r="W12" s="1">
         <f t="shared" si="5"/>
@@ -2193,7 +2192,7 @@
       <c r="I13" t="s">
         <v>98</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="1">
         <f t="shared" si="8"/>
         <v>44593</v>
       </c>
@@ -2236,7 +2235,7 @@
       </c>
       <c r="V13">
         <f t="shared" ca="1" si="4"/>
-        <v>899707</v>
+        <v>2939185</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" si="5"/>
@@ -2308,7 +2307,7 @@
       <c r="I14" t="s">
         <v>98</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="1">
         <f t="shared" si="8"/>
         <v>44593</v>
       </c>
@@ -2351,7 +2350,7 @@
       </c>
       <c r="V14">
         <f t="shared" ca="1" si="4"/>
-        <v>648554</v>
+        <v>757208</v>
       </c>
       <c r="W14" s="1">
         <f t="shared" si="5"/>
@@ -2423,7 +2422,7 @@
       <c r="I15" t="s">
         <v>98</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -2466,7 +2465,7 @@
       </c>
       <c r="V15">
         <f t="shared" ca="1" si="4"/>
-        <v>2117564</v>
+        <v>2218108</v>
       </c>
       <c r="W15" s="1">
         <f t="shared" si="5"/>
@@ -2542,7 +2541,7 @@
       <c r="I16" t="s">
         <v>98</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -2585,7 +2584,7 @@
       </c>
       <c r="V16">
         <f t="shared" ca="1" si="4"/>
-        <v>665165</v>
+        <v>1173524</v>
       </c>
       <c r="W16" s="1">
         <f t="shared" si="5"/>
@@ -2657,7 +2656,7 @@
       <c r="I17" t="s">
         <v>98</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -2698,7 +2697,7 @@
         <f>DATE(YEAR(S17)+2, MONTH(S17), DAY(S17))</f>
         <v>45292</v>
       </c>
-      <c r="V17" s="4">
+      <c r="V17" s="3">
         <v>351822</v>
       </c>
       <c r="W17" s="1">
@@ -2771,7 +2770,7 @@
       <c r="I18" t="s">
         <v>98</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -2889,7 +2888,7 @@
       <c r="I19" t="s">
         <v>98</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -3007,7 +3006,7 @@
       <c r="I20" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -3125,7 +3124,7 @@
       <c r="I21" t="s">
         <v>98</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="1">
         <f t="shared" si="7"/>
         <v>44927</v>
       </c>
@@ -3239,7 +3238,7 @@
       <c r="I22" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="1">
         <f t="shared" ref="J22:J28" si="13">DATE(YEAR(S22)+1,MONTH(S22),DAY(S22))</f>
         <v>44927</v>
       </c>
@@ -3353,7 +3352,7 @@
       <c r="I23" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="1">
         <f t="shared" si="13"/>
         <v>44927</v>
       </c>
@@ -3471,7 +3470,7 @@
       <c r="I24" t="s">
         <v>98</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="1">
         <f t="shared" si="13"/>
         <v>44927</v>
       </c>
@@ -3589,7 +3588,7 @@
       <c r="I25" t="s">
         <v>98</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="1">
         <f t="shared" si="13"/>
         <v>44927</v>
       </c>
@@ -3630,7 +3629,7 @@
         <f>DATE(YEAR(S25)+10, MONTH(S25), DAY(S25))</f>
         <v>48214</v>
       </c>
-      <c r="V25" s="4">
+      <c r="V25" s="3">
         <v>3500000</v>
       </c>
       <c r="W25" s="1">
@@ -3707,7 +3706,7 @@
       <c r="I26" t="s">
         <v>98</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="1">
         <f t="shared" si="13"/>
         <v>44927</v>
       </c>
@@ -3821,7 +3820,7 @@
       <c r="I27" t="s">
         <v>98</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="1">
         <f t="shared" si="13"/>
         <v>44927</v>
       </c>
@@ -3935,7 +3934,7 @@
       <c r="I28" t="s">
         <v>98</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="1">
         <f t="shared" si="13"/>
         <v>44927</v>
       </c>

</xml_diff>

<commit_message>
Implement Equity and Liquidity Coverage ratio methods in Value.R Update data to start without a MarketObject
</commit_message>
<xml_diff>
--- a/src/data/bankA/ANN_Portfolio.xlsx
+++ b/src/data/bankA/ANN_Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/bankA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8716DF2-6240-A84B-8965-EA426418246E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D616A2-613F-EA49-8CA5-7D9217EF00A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{2827F415-5853-FE46-AE22-EC4475DFFC5F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="101">
   <si>
     <t>calendar</t>
   </si>
@@ -339,9 +339,6 @@
   </si>
   <si>
     <t>3 years loan to bank with variable rate + spread</t>
-  </si>
-  <si>
-    <t>YC_CTRS</t>
   </si>
 </sst>
 </file>
@@ -707,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF54409-75AA-D240-BC62-D87145E7C900}">
   <dimension ref="A1:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V28"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -933,7 +930,7 @@
       </c>
       <c r="V2" s="3">
         <f ca="1">RANDBETWEEN(500000, 3000000)</f>
-        <v>2952871</v>
+        <v>2827448</v>
       </c>
       <c r="W2" s="1">
         <f>DATE(YEAR(S2)+1,MONTH(S2),DAY(S2))</f>
@@ -948,18 +945,9 @@
       <c r="Z2" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="1">
-        <f>R2</f>
-        <v>44561</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>101</v>
+      <c r="AA2" s="1"/>
+      <c r="AC2">
+        <v>0</v>
       </c>
       <c r="AE2" t="s">
         <v>44</v>
@@ -1052,7 +1040,7 @@
       </c>
       <c r="V3" s="3">
         <f t="shared" ref="V3:V16" ca="1" si="4">RANDBETWEEN(500000, 3000000)</f>
-        <v>1160480</v>
+        <v>1353936</v>
       </c>
       <c r="W3" s="1">
         <f t="shared" ref="W3:W16" si="5">DATE(YEAR(S3)+1,MONTH(S3),DAY(S3))</f>
@@ -1067,18 +1055,9 @@
       <c r="Z3" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="1">
-        <f t="shared" ref="AA3:AA15" si="6">R3</f>
-        <v>44561</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>101</v>
+      <c r="AA3" s="1"/>
+      <c r="AC3">
+        <v>0</v>
       </c>
       <c r="AE3" t="s">
         <v>44</v>
@@ -1129,7 +1108,7 @@
         <v>94</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J28" si="7">DATE(YEAR(S4)+1,MONTH(S4),DAY(S4))</f>
+        <f t="shared" ref="J4:J28" si="6">DATE(YEAR(S4)+1,MONTH(S4),DAY(S4))</f>
         <v>44927</v>
       </c>
       <c r="K4" t="s">
@@ -1171,7 +1150,7 @@
       </c>
       <c r="V4" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>526197</v>
+        <v>1901324</v>
       </c>
       <c r="W4" s="1">
         <f t="shared" si="5"/>
@@ -1186,18 +1165,9 @@
       <c r="Z4" t="s">
         <v>37</v>
       </c>
-      <c r="AA4" s="1">
-        <f t="shared" si="6"/>
-        <v>44561</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>101</v>
+      <c r="AA4" s="1"/>
+      <c r="AC4">
+        <v>0</v>
       </c>
       <c r="AE4" t="s">
         <v>44</v>
@@ -1248,7 +1218,7 @@
         <v>94</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K5" t="s">
@@ -1290,7 +1260,7 @@
       </c>
       <c r="V5" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>1793116</v>
+        <v>1646000</v>
       </c>
       <c r="W5" s="1">
         <f t="shared" si="5"/>
@@ -1305,17 +1275,9 @@
       <c r="Z5" t="s">
         <v>37</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>37</v>
+      <c r="AA5" s="1"/>
+      <c r="AC5">
+        <v>0</v>
       </c>
       <c r="AE5" t="s">
         <v>44</v>
@@ -1366,7 +1328,7 @@
         <v>94</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K6" t="s">
@@ -1408,7 +1370,7 @@
       </c>
       <c r="V6" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>1382899</v>
+        <v>2805810</v>
       </c>
       <c r="W6" s="1">
         <f t="shared" si="5"/>
@@ -1423,17 +1385,9 @@
       <c r="Z6" t="s">
         <v>37</v>
       </c>
-      <c r="AA6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>37</v>
+      <c r="AA6" s="1"/>
+      <c r="AC6">
+        <v>0</v>
       </c>
       <c r="AE6" t="s">
         <v>44</v>
@@ -1484,7 +1438,7 @@
         <v>94</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K7" t="s">
@@ -1526,7 +1480,7 @@
       </c>
       <c r="V7" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2084005</v>
+        <v>1537278</v>
       </c>
       <c r="W7" s="1">
         <f t="shared" si="5"/>
@@ -1541,17 +1495,9 @@
       <c r="Z7" t="s">
         <v>37</v>
       </c>
-      <c r="AA7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>37</v>
+      <c r="AA7" s="1"/>
+      <c r="AC7">
+        <v>0</v>
       </c>
       <c r="AE7" t="s">
         <v>44</v>
@@ -1602,7 +1548,7 @@
         <v>94</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K8" t="s">
@@ -1644,7 +1590,7 @@
       </c>
       <c r="V8" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>719439</v>
+        <v>1039159</v>
       </c>
       <c r="W8" s="1">
         <f t="shared" si="5"/>
@@ -1659,18 +1605,9 @@
       <c r="Z8" t="s">
         <v>37</v>
       </c>
-      <c r="AA8" s="1">
-        <f t="shared" si="6"/>
-        <v>44561</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA8" s="1"/>
       <c r="AC8">
-        <v>0.04</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="s">
         <v>44</v>
@@ -1721,7 +1658,7 @@
         <v>94</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K9" t="s">
@@ -1763,7 +1700,7 @@
       </c>
       <c r="V9" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>1684805</v>
+        <v>2586410</v>
       </c>
       <c r="W9" s="1">
         <f t="shared" si="5"/>
@@ -1778,18 +1715,9 @@
       <c r="Z9" t="s">
         <v>37</v>
       </c>
-      <c r="AA9" s="1">
-        <f t="shared" si="6"/>
-        <v>44561</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA9" s="1"/>
       <c r="AC9">
-        <v>0.04</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE9" t="s">
         <v>44</v>
@@ -1840,7 +1768,7 @@
         <v>94</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K10" t="s">
@@ -1882,7 +1810,7 @@
       </c>
       <c r="V10" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2583268</v>
+        <v>2211751</v>
       </c>
       <c r="W10" s="1">
         <f t="shared" si="5"/>
@@ -1897,17 +1825,9 @@
       <c r="Z10" t="s">
         <v>37</v>
       </c>
-      <c r="AA10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>37</v>
-      </c>
+      <c r="AA10" s="1"/>
       <c r="AC10">
-        <v>0.04</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="s">
         <v>44</v>
@@ -1958,7 +1878,7 @@
         <v>94</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K11" t="s">
@@ -2000,7 +1920,7 @@
       </c>
       <c r="V11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>693912</v>
+        <v>1137489</v>
       </c>
       <c r="W11" s="1">
         <f t="shared" si="5"/>
@@ -2015,18 +1935,9 @@
       <c r="Z11" t="s">
         <v>37</v>
       </c>
-      <c r="AA11" s="1">
-        <f t="shared" si="6"/>
-        <v>44561</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA11" s="1"/>
       <c r="AC11">
-        <v>0.05</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="s">
         <v>44</v>
@@ -2077,7 +1988,7 @@
         <v>94</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K12" t="s">
@@ -2119,7 +2030,7 @@
       </c>
       <c r="V12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>542812</v>
+        <v>2018925</v>
       </c>
       <c r="W12" s="1">
         <f t="shared" si="5"/>
@@ -2134,18 +2045,9 @@
       <c r="Z12" t="s">
         <v>37</v>
       </c>
-      <c r="AA12" s="1">
-        <f t="shared" si="6"/>
-        <v>44561</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA12" s="1"/>
       <c r="AC12">
-        <v>0.06</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE12" t="s">
         <v>44</v>
@@ -2196,7 +2098,7 @@
         <v>94</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K13" t="s">
@@ -2238,7 +2140,7 @@
       </c>
       <c r="V13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>1873304</v>
+        <v>2840183</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" si="5"/>
@@ -2253,17 +2155,9 @@
       <c r="Z13" t="s">
         <v>37</v>
       </c>
-      <c r="AA13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>37</v>
-      </c>
+      <c r="AA13" s="1"/>
       <c r="AC13">
-        <v>0.05</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AE13" t="s">
         <v>44</v>
@@ -2314,7 +2208,7 @@
         <v>94</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K14" t="s">
@@ -2356,7 +2250,7 @@
       </c>
       <c r="V14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2883905</v>
+        <v>1204752</v>
       </c>
       <c r="W14" s="1">
         <f t="shared" si="5"/>
@@ -2371,17 +2265,9 @@
       <c r="Z14" t="s">
         <v>37</v>
       </c>
-      <c r="AA14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>37</v>
-      </c>
+      <c r="AA14" s="1"/>
       <c r="AC14">
-        <v>0.06</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="AE14" t="s">
         <v>44</v>
@@ -2432,7 +2318,7 @@
         <v>94</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K15" t="s">
@@ -2474,7 +2360,7 @@
       </c>
       <c r="V15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2359243</v>
+        <v>1845827</v>
       </c>
       <c r="W15" s="1">
         <f t="shared" si="5"/>
@@ -2489,18 +2375,9 @@
       <c r="Z15" t="s">
         <v>37</v>
       </c>
-      <c r="AA15" s="1">
-        <f t="shared" si="6"/>
-        <v>44561</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>101</v>
+      <c r="AA15" s="1"/>
+      <c r="AC15">
+        <v>0</v>
       </c>
       <c r="AE15" t="s">
         <v>44</v>
@@ -2551,7 +2428,7 @@
         <v>94</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K16" t="s">
@@ -2593,7 +2470,7 @@
       </c>
       <c r="V16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>1241887</v>
+        <v>1619621</v>
       </c>
       <c r="W16" s="1">
         <f t="shared" si="5"/>
@@ -2608,17 +2485,9 @@
       <c r="Z16" t="s">
         <v>37</v>
       </c>
-      <c r="AA16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC16" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>37</v>
+      <c r="AA16" s="1"/>
+      <c r="AC16">
+        <v>0</v>
       </c>
       <c r="AE16" t="s">
         <v>44</v>
@@ -2669,7 +2538,7 @@
         <v>94</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K17" t="s">
@@ -2691,11 +2560,11 @@
         <v>43</v>
       </c>
       <c r="Q17" s="1">
-        <f t="shared" ref="Q17:Q28" si="8">U17</f>
+        <f t="shared" ref="Q17:Q28" si="7">U17</f>
         <v>45292</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" ref="R17:R23" si="9">E17</f>
+        <f t="shared" ref="R17:R23" si="8">E17</f>
         <v>44561</v>
       </c>
       <c r="S17" s="1">
@@ -2725,17 +2594,9 @@
       <c r="Z17" t="s">
         <v>37</v>
       </c>
-      <c r="AA17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>37</v>
+      <c r="AA17" s="1"/>
+      <c r="AC17">
+        <v>0</v>
       </c>
       <c r="AE17" t="s">
         <v>44</v>
@@ -2786,7 +2647,7 @@
         <v>94</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K18" t="s">
@@ -2808,11 +2669,11 @@
         <v>43</v>
       </c>
       <c r="Q18" s="1">
+        <f t="shared" si="7"/>
+        <v>46388</v>
+      </c>
+      <c r="R18" s="1">
         <f t="shared" si="8"/>
-        <v>46388</v>
-      </c>
-      <c r="R18" s="1">
-        <f t="shared" si="9"/>
         <v>44561</v>
       </c>
       <c r="S18" s="1">
@@ -2830,7 +2691,7 @@
         <v>550000</v>
       </c>
       <c r="W18" s="1">
-        <f t="shared" ref="W18:W23" si="10">DATE(YEAR(S18)+1,MONTH(S18),DAY(S18))</f>
+        <f t="shared" ref="W18:W23" si="9">DATE(YEAR(S18)+1,MONTH(S18),DAY(S18))</f>
         <v>44927</v>
       </c>
       <c r="X18" t="s">
@@ -2842,18 +2703,9 @@
       <c r="Z18" t="s">
         <v>37</v>
       </c>
-      <c r="AA18" s="1">
-        <f t="shared" ref="AA18:AA20" si="11">R18</f>
-        <v>44561</v>
-      </c>
-      <c r="AB18" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD18" t="s">
-        <v>101</v>
+      <c r="AA18" s="1"/>
+      <c r="AC18">
+        <v>0</v>
       </c>
       <c r="AE18" t="s">
         <v>44</v>
@@ -2904,7 +2756,7 @@
         <v>94</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K19" t="s">
@@ -2926,11 +2778,11 @@
         <v>43</v>
       </c>
       <c r="Q19" s="1">
+        <f t="shared" si="7"/>
+        <v>46023</v>
+      </c>
+      <c r="R19" s="1">
         <f t="shared" si="8"/>
-        <v>46023</v>
-      </c>
-      <c r="R19" s="1">
-        <f t="shared" si="9"/>
         <v>44561</v>
       </c>
       <c r="S19" s="1">
@@ -2948,7 +2800,7 @@
         <v>725000</v>
       </c>
       <c r="W19" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>44927</v>
       </c>
       <c r="X19" t="s">
@@ -2960,18 +2812,9 @@
       <c r="Z19" t="s">
         <v>37</v>
       </c>
-      <c r="AA19" s="1">
-        <f t="shared" si="11"/>
-        <v>44561</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA19" s="1"/>
       <c r="AC19">
-        <v>0.02</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE19" t="s">
         <v>44</v>
@@ -3022,7 +2865,7 @@
         <v>94</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K20" t="s">
@@ -3044,11 +2887,11 @@
         <v>43</v>
       </c>
       <c r="Q20" s="1">
+        <f t="shared" si="7"/>
+        <v>47119</v>
+      </c>
+      <c r="R20" s="1">
         <f t="shared" si="8"/>
-        <v>47119</v>
-      </c>
-      <c r="R20" s="1">
-        <f t="shared" si="9"/>
         <v>44561</v>
       </c>
       <c r="S20" s="1">
@@ -3066,7 +2909,7 @@
         <v>225000</v>
       </c>
       <c r="W20" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>44927</v>
       </c>
       <c r="X20" t="s">
@@ -3078,18 +2921,9 @@
       <c r="Z20" t="s">
         <v>37</v>
       </c>
-      <c r="AA20" s="1">
-        <f t="shared" si="11"/>
-        <v>44561</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA20" s="1"/>
       <c r="AC20">
-        <v>0.03</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE20" t="s">
         <v>44</v>
@@ -3140,7 +2974,7 @@
         <v>94</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K21" t="s">
@@ -3162,11 +2996,11 @@
         <v>43</v>
       </c>
       <c r="Q21" s="1">
+        <f t="shared" si="7"/>
+        <v>46753</v>
+      </c>
+      <c r="R21" s="1">
         <f t="shared" si="8"/>
-        <v>46753</v>
-      </c>
-      <c r="R21" s="1">
-        <f t="shared" si="9"/>
         <v>44561</v>
       </c>
       <c r="S21" s="1">
@@ -3184,7 +3018,7 @@
         <v>500000</v>
       </c>
       <c r="W21" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>44927</v>
       </c>
       <c r="X21" t="s">
@@ -3196,17 +3030,9 @@
       <c r="Z21" t="s">
         <v>37</v>
       </c>
-      <c r="AA21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>37</v>
+      <c r="AA21" s="1"/>
+      <c r="AC21">
+        <v>0</v>
       </c>
       <c r="AE21" t="s">
         <v>44</v>
@@ -3257,7 +3083,7 @@
         <v>94</v>
       </c>
       <c r="J22" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K22" t="s">
@@ -3279,11 +3105,11 @@
         <v>43</v>
       </c>
       <c r="Q22" s="1">
+        <f t="shared" si="7"/>
+        <v>48214</v>
+      </c>
+      <c r="R22" s="1">
         <f t="shared" si="8"/>
-        <v>48214</v>
-      </c>
-      <c r="R22" s="1">
-        <f t="shared" si="9"/>
         <v>44561</v>
       </c>
       <c r="S22" s="1">
@@ -3301,7 +3127,7 @@
         <v>1450000</v>
       </c>
       <c r="W22" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>44927</v>
       </c>
       <c r="X22" t="s">
@@ -3313,17 +3139,9 @@
       <c r="Z22" t="s">
         <v>37</v>
       </c>
-      <c r="AA22" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC22" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>37</v>
+      <c r="AA22" s="1"/>
+      <c r="AC22">
+        <v>0</v>
       </c>
       <c r="AE22" t="s">
         <v>44</v>
@@ -3374,7 +3192,7 @@
         <v>94</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K23" t="s">
@@ -3396,11 +3214,11 @@
         <v>43</v>
       </c>
       <c r="Q23" s="1">
+        <f t="shared" si="7"/>
+        <v>47484</v>
+      </c>
+      <c r="R23" s="1">
         <f t="shared" si="8"/>
-        <v>47484</v>
-      </c>
-      <c r="R23" s="1">
-        <f t="shared" si="9"/>
         <v>44561</v>
       </c>
       <c r="S23" s="1">
@@ -3418,7 +3236,7 @@
         <v>550000</v>
       </c>
       <c r="W23" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>44927</v>
       </c>
       <c r="X23" t="s">
@@ -3430,18 +3248,9 @@
       <c r="Z23" t="s">
         <v>37</v>
       </c>
-      <c r="AA23" s="1">
-        <f t="shared" ref="AA23:AA25" si="12">R23</f>
-        <v>44561</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA23" s="1"/>
       <c r="AC23">
-        <v>0.01</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE23" t="s">
         <v>44</v>
@@ -3492,7 +3301,7 @@
         <v>94</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K24" t="s">
@@ -3514,11 +3323,11 @@
         <v>43</v>
       </c>
       <c r="Q24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>46388</v>
       </c>
       <c r="R24" s="1">
-        <f t="shared" ref="R24:R28" si="13">E24</f>
+        <f t="shared" ref="R24:R28" si="10">E24</f>
         <v>44561</v>
       </c>
       <c r="S24" s="1">
@@ -3536,7 +3345,7 @@
         <v>1500000</v>
       </c>
       <c r="W24" s="1">
-        <f t="shared" ref="W24:W28" si="14">DATE(YEAR(S24)+1,MONTH(S24),DAY(S24))</f>
+        <f t="shared" ref="W24:W28" si="11">DATE(YEAR(S24)+1,MONTH(S24),DAY(S24))</f>
         <v>44927</v>
       </c>
       <c r="X24" t="s">
@@ -3548,18 +3357,9 @@
       <c r="Z24" t="s">
         <v>37</v>
       </c>
-      <c r="AA24" s="1">
-        <f t="shared" si="12"/>
-        <v>44561</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA24" s="1"/>
       <c r="AC24">
-        <v>0.02</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE24" t="s">
         <v>44</v>
@@ -3610,7 +3410,7 @@
         <v>94</v>
       </c>
       <c r="J25" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K25" t="s">
@@ -3632,11 +3432,11 @@
         <v>43</v>
       </c>
       <c r="Q25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>48214</v>
       </c>
       <c r="R25" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S25" s="1">
@@ -3654,7 +3454,7 @@
         <v>3500000</v>
       </c>
       <c r="W25" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X25" t="s">
@@ -3666,18 +3466,9 @@
       <c r="Z25" t="s">
         <v>37</v>
       </c>
-      <c r="AA25" s="1">
-        <f t="shared" si="12"/>
-        <v>44561</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA25" s="1"/>
       <c r="AC25">
-        <v>0.03</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE25" t="s">
         <v>44</v>
@@ -3728,7 +3519,7 @@
         <v>94</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K26" t="s">
@@ -3750,11 +3541,11 @@
         <v>43</v>
       </c>
       <c r="Q26" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>47119</v>
       </c>
       <c r="R26" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S26" s="1">
@@ -3772,7 +3563,7 @@
         <v>2000000</v>
       </c>
       <c r="W26" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X26" t="s">
@@ -3784,17 +3575,9 @@
       <c r="Z26" t="s">
         <v>37</v>
       </c>
-      <c r="AA26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>37</v>
+      <c r="AA26" s="1"/>
+      <c r="AC26">
+        <v>0</v>
       </c>
       <c r="AE26" t="s">
         <v>44</v>
@@ -3845,7 +3628,7 @@
         <v>94</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K27" t="s">
@@ -3867,11 +3650,11 @@
         <v>43</v>
       </c>
       <c r="Q27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>45292</v>
       </c>
       <c r="R27" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S27" s="1">
@@ -3889,7 +3672,7 @@
         <v>1250000</v>
       </c>
       <c r="W27" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X27" t="s">
@@ -3901,17 +3684,9 @@
       <c r="Z27" t="s">
         <v>37</v>
       </c>
-      <c r="AA27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>37</v>
+      <c r="AA27" s="1"/>
+      <c r="AC27">
+        <v>0</v>
       </c>
       <c r="AE27" t="s">
         <v>44</v>
@@ -3962,7 +3737,7 @@
         <v>94</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>44927</v>
       </c>
       <c r="K28" t="s">
@@ -3984,11 +3759,11 @@
         <v>43</v>
       </c>
       <c r="Q28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>45658</v>
       </c>
       <c r="R28" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>44561</v>
       </c>
       <c r="S28" s="1">
@@ -4006,7 +3781,7 @@
         <v>1750000</v>
       </c>
       <c r="W28" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>44927</v>
       </c>
       <c r="X28" t="s">
@@ -4018,18 +3793,9 @@
       <c r="Z28" t="s">
         <v>37</v>
       </c>
-      <c r="AA28" s="1">
-        <f t="shared" ref="AA28" si="15">R28</f>
-        <v>44561</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>59</v>
-      </c>
+      <c r="AA28" s="1"/>
       <c r="AC28">
-        <v>0.01</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="AE28" t="s">
         <v>44</v>

</xml_diff>